<commit_message>
Updated account creation page
</commit_message>
<xml_diff>
--- a/E-commerceApp/src/test/resources/TestData/TestData.xlsx
+++ b/E-commerceApp/src/test/resources/TestData/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="98">
   <si>
     <t xml:space="preserve">Smoke</t>
   </si>
@@ -191,7 +191,7 @@
     <t xml:space="preserve">Email</t>
   </si>
   <si>
-    <t xml:space="preserve">itanilkumar05@gmail.com</t>
+    <t xml:space="preserve">anilkumar@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Product</t>
@@ -251,7 +251,7 @@
     <t xml:space="preserve">MobilePhone</t>
   </si>
   <si>
-    <t xml:space="preserve">newtest1@gmail.com</t>
+    <t xml:space="preserve">fsfsfdsf@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Mrs</t>
@@ -263,7 +263,7 @@
     <t xml:space="preserve">UserTest</t>
   </si>
   <si>
-    <t xml:space="preserve">hgsdtyf</t>
+    <t xml:space="preserve">test@123</t>
   </si>
   <si>
     <t xml:space="preserve">22</t>
@@ -275,10 +275,10 @@
     <t xml:space="preserve">1985</t>
   </si>
   <si>
-    <t xml:space="preserve">ABCDEF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EDFG123</t>
+    <t xml:space="preserve">meslova</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hytech</t>
   </si>
   <si>
     <t xml:space="preserve">San</t>
@@ -293,13 +293,37 @@
     <t xml:space="preserve">United States</t>
   </si>
   <si>
-    <t xml:space="preserve">8489875678</t>
-  </si>
-  <si>
-    <t xml:space="preserve">newtest2@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">newtest3@gmail.com</t>
+    <t xml:space="preserve">9556238894</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agwv@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test@124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">madhpur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7077777607</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfdagwv@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test@125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ammerpet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9777997046</t>
   </si>
 </sst>
 </file>
@@ -558,7 +582,7 @@
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.71"/>
@@ -826,7 +850,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.29"/>
@@ -873,11 +897,11 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.57"/>
   </cols>
@@ -894,7 +918,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="itanilkumar05@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="anilkumar@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -917,7 +941,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -963,7 +987,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -993,15 +1017,15 @@
   </sheetPr>
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.29"/>
@@ -1062,7 +1086,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
         <v>73</v>
       </c>
@@ -1109,7 +1133,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
         <v>88</v>
       </c>
@@ -1123,7 +1147,7 @@
         <v>76</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>78</v>
@@ -1135,10 +1159,10 @@
         <v>80</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="K3" s="12" t="s">
         <v>83</v>
@@ -1153,12 +1177,12 @@
         <v>86</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>74</v>
@@ -1170,7 +1194,7 @@
         <v>76</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>78</v>
@@ -1182,10 +1206,10 @@
         <v>80</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="K4" s="12" t="s">
         <v>83</v>
@@ -1200,14 +1224,15 @@
         <v>86</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="newtest1@gmail.com"/>
-    <hyperlink ref="A3" r:id="rId2" display="newtest2@gmail.com"/>
-    <hyperlink ref="A4" r:id="rId3" display="newtest3@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="fsfsfdsf@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId2" display="test@123"/>
+    <hyperlink ref="A3" r:id="rId3" display="agwv@gmail.com"/>
+    <hyperlink ref="A4" r:id="rId4" display="dfdagwv@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>